<commit_message>
Von Gruppe 2 gefundene Fehler eingefügt
</commit_message>
<xml_diff>
--- a/additional/WiSe13/fehlerListe_WiSe13.xlsx
+++ b/additional/WiSe13/fehlerListe_WiSe13.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\padberg\git\wppetrinetze\additional\WiSe13\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6825"/>
   </bookViews>
@@ -17,9 +12,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>F001</t>
   </si>
@@ -78,13 +73,34 @@
   </si>
   <si>
     <t>Fehlergewicht                                 1 (harmlos)-6 (katastrophal)</t>
+  </si>
+  <si>
+    <t>F003</t>
+  </si>
+  <si>
+    <t>F004</t>
+  </si>
+  <si>
+    <t>Dalock/Bauß</t>
+  </si>
+  <si>
+    <t>im Verzeichnis F003_F004</t>
+  </si>
+  <si>
+    <t>im Verzeichnis F003_F005</t>
+  </si>
+  <si>
+    <t>Stellen/Transitionen lassen sich in der GUI (Im Regel-Fenster) untereinander schieben</t>
+  </si>
+  <si>
+    <t>Beim Löschen eines Elementes aus der GUI wird, wenn man danach einen Rechtsklick ausführt eine oder mehrere Exceptions geworfen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,7 +212,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,7 +247,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,24 +424,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -438,7 +454,7 @@
     <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -467,7 +483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" customHeight="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -487,7 +503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30" customHeight="1">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -507,22 +523,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:9" ht="30" customHeight="1">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1"/>
+    <row r="7" spans="1:9" ht="30" customHeight="1"/>
+    <row r="8" spans="1:9" ht="30" customHeight="1"/>
+    <row r="9" spans="1:9" ht="30" customHeight="1"/>
+    <row r="10" spans="1:9" ht="30" customHeight="1"/>
+    <row r="11" spans="1:9" ht="30" customHeight="1"/>
+    <row r="12" spans="1:9" ht="30" customHeight="1"/>
+    <row r="13" spans="1:9" ht="30" customHeight="1"/>
+    <row r="14" spans="1:9" ht="30" customHeight="1"/>
+    <row r="15" spans="1:9" ht="30" customHeight="1"/>
+    <row r="16" spans="1:9" ht="30" customHeight="1"/>
+    <row r="17" ht="30" customHeight="1"/>
+    <row r="18" ht="30" customHeight="1"/>
+    <row r="19" ht="30" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <printOptions gridLines="1"/>

</xml_diff>